<commit_message>
issue tracker excel sheet
</commit_message>
<xml_diff>
--- a/CMS_Issue_List_23-11-2017.xlsx
+++ b/CMS_Issue_List_23-11-2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="18" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="18" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="16-06-2017" sheetId="1" r:id="rId1"/>
@@ -1450,16 +1450,10 @@
     <t>booth level--&gt; templete</t>
   </si>
   <si>
-    <t xml:space="preserve">                                   CMS WEB TESTING REPORT OF NEW FEATURE AS BOOTH LEVEL IN BULCKUPLOAD</t>
-  </si>
-  <si>
     <t>should be mentoined as  door number field  starts with "#" in templete</t>
   </si>
   <si>
     <t xml:space="preserve">                                        url link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                   CMS WEB TESTING REPORT OF NEW FEATURE AS REGISTERATION AND REPORTS MODULE</t>
   </si>
   <si>
     <t>Search box</t>
@@ -1469,9 +1463,6 @@
 membership id ,age ,name fields are  not working in  search box</t>
   </si>
   <si>
-    <t>if you search particular mobile details,then  click on download button it should not download the overall data,But it's downloading all.</t>
-  </si>
-  <si>
     <t>http://202.153.34.166:8001/campaign/boothstatus</t>
   </si>
   <si>
@@ -1536,6 +1527,15 @@
   </si>
   <si>
     <t>booth number field is missing in registeration page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   CMS WEB TESTING REPORT OF NEW FEATURE OF REGISTERATION AND REPORTS MODULE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   CMS WEB TESTING REPORT OF NEW FEATURE OF BOOTH LEVEL IN BULCKUPLOAD</t>
+  </si>
+  <si>
+    <t>if you search particular mobile details,then  click on download button it should not download the pareticular data,But it's downloading all.</t>
   </si>
 </sst>
 </file>
@@ -6264,8 +6264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6281,7 +6281,7 @@
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
       <c r="C1" s="38" t="s">
-        <v>453</v>
+        <v>480</v>
       </c>
       <c r="D1" s="38"/>
       <c r="E1" s="38"/>
@@ -6302,7 +6302,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F2" s="39" t="s">
         <v>4</v>
@@ -6362,7 +6362,7 @@
         <v>271</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
@@ -6373,7 +6373,7 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B6" t="s">
         <v>421</v>
@@ -6382,10 +6382,10 @@
         <v>271</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E6" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -6393,7 +6393,7 @@
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B7" t="s">
         <v>421</v>
@@ -6402,10 +6402,10 @@
         <v>271</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E7" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -6431,8 +6431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6450,7 +6450,7 @@
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
       <c r="C1" s="38" t="s">
-        <v>456</v>
+        <v>479</v>
       </c>
       <c r="D1" s="38"/>
       <c r="E1" s="38"/>
@@ -6465,13 +6465,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D2" s="39" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F2" s="39" t="s">
         <v>4</v>
@@ -6485,19 +6485,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C3" s="45" t="s">
         <v>183</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E3" t="s">
         <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6511,18 +6511,18 @@
         <v>183</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
-        <v>10</v>
+      <c r="F4" s="49" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B5" t="s">
         <v>75</v>
@@ -6531,13 +6531,13 @@
         <v>183</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
-        <v>10</v>
+      <c r="F5" s="49" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6545,19 +6545,19 @@
         <v>368</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C6" s="45" t="s">
         <v>370</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E6" t="s">
         <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6571,13 +6571,13 @@
         <v>370</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>459</v>
+        <v>481</v>
       </c>
       <c r="E7" t="s">
         <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -6585,19 +6585,19 @@
         <v>368</v>
       </c>
       <c r="B8" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -6605,79 +6605,79 @@
         <v>368</v>
       </c>
       <c r="B9" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E9" t="s">
         <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B10" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C10" s="45" t="s">
         <v>370</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="E10" t="s">
         <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B11" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C11" s="47" t="s">
+        <v>464</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>467</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>470</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
-        <v>10</v>
+      <c r="F11" s="49" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B12" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C12" s="45" t="s">
         <v>183</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E12" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>